<commit_message>
committing all the little files that probably don't need to be committed but I need to push them from my local so I can open the -gr branch! Note- need to learn how to untrack certain files!
</commit_message>
<xml_diff>
--- a/data/number_daily_exceedances_pm10_trs.xlsx
+++ b/data/number_daily_exceedances_pm10_trs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R_working_directory\pg-aqmp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA2BC8DA-5A0E-47E2-9D05-E075F4880621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D9D138D-B71E-4541-ADAD-85BAB6FCA0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="16330" windowHeight="9200" xr2:uid="{BF91BB17-A3CB-427C-9463-E8B24D3D6E96}"/>
+    <workbookView xWindow="1140" yWindow="1000" windowWidth="16330" windowHeight="9200" xr2:uid="{BF91BB17-A3CB-427C-9463-E8B24D3D6E96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="11">
   <si>
     <t>year</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>hr</t>
+  </si>
+  <si>
+    <t>data_capture</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -121,6 +130,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,15 +453,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C540807-B716-43A1-BE0D-C396B96EE789}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,8 +474,11 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>2010</v>
       </c>
@@ -475,8 +491,11 @@
       <c r="D2" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2011</v>
       </c>
@@ -489,8 +508,11 @@
       <c r="D3" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2012</v>
       </c>
@@ -503,8 +525,11 @@
       <c r="D4" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2013</v>
       </c>
@@ -517,8 +542,11 @@
       <c r="D5" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2014</v>
       </c>
@@ -531,8 +559,11 @@
       <c r="D6" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2015</v>
       </c>
@@ -545,8 +576,11 @@
       <c r="D7" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2016</v>
       </c>
@@ -559,8 +593,11 @@
       <c r="D8" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>2017</v>
       </c>
@@ -573,8 +610,11 @@
       <c r="D9" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>2018</v>
       </c>
@@ -587,8 +627,11 @@
       <c r="D10" s="1">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>2019</v>
       </c>
@@ -601,8 +644,11 @@
       <c r="D11" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>2020</v>
       </c>
@@ -615,8 +661,11 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>2021</v>
       </c>
@@ -629,8 +678,11 @@
       <c r="D13" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>2022</v>
       </c>
@@ -643,8 +695,11 @@
       <c r="D14" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>2023</v>
       </c>
@@ -657,551 +712,745 @@
       <c r="D15" s="1">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
         <v>2010</v>
       </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1">
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1">
         <v>123</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
         <v>2011</v>
       </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
         <v>2012</v>
       </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1">
         <v>123</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
         <v>2013</v>
       </c>
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="1">
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1">
         <v>116</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="1">
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
         <v>2014</v>
       </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1">
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1">
         <v>146</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
         <v>2015</v>
       </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="1">
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="1">
         <v>114</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="1">
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
         <v>2016</v>
       </c>
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="1">
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="1">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
         <v>2017</v>
       </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="1">
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1">
         <v>84</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="1">
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
         <v>2018</v>
       </c>
-      <c r="B24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="1">
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="1">
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
         <v>2019</v>
       </c>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="1">
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1">
         <v>69</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="1">
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
         <v>2020</v>
       </c>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="1">
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="1">
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
         <v>2021</v>
       </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="1">
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="1">
         <v>67</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="1">
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
         <v>2022</v>
       </c>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="1">
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1">
         <v>70</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="1">
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
         <v>2023</v>
       </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="1">
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1">
         <v>112</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="1">
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="1">
+        <v>82</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
         <v>2010</v>
       </c>
-      <c r="B30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="1">
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
         <v>2011</v>
       </c>
-      <c r="B31" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="1">
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
         <v>2012</v>
       </c>
-      <c r="B32" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="1">
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
         <v>2013</v>
       </c>
-      <c r="B33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="1">
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
         <v>2014</v>
       </c>
-      <c r="B34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="1">
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
         <v>2015</v>
       </c>
-      <c r="B35" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="1">
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
         <v>2016</v>
       </c>
-      <c r="B36" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="1">
+      <c r="B38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
         <v>2017</v>
       </c>
-      <c r="B37" t="s">
-        <v>2</v>
-      </c>
-      <c r="C37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="1">
+      <c r="B39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
         <v>2018</v>
       </c>
-      <c r="B38" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="1">
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="1">
         <v>2019</v>
       </c>
-      <c r="B39" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="1">
+      <c r="B41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="1">
         <v>2020</v>
       </c>
-      <c r="B40" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="1">
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="1">
         <v>2021</v>
       </c>
-      <c r="B41" t="s">
-        <v>2</v>
-      </c>
-      <c r="C41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="1">
+      <c r="B43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="1">
         <v>2022</v>
       </c>
-      <c r="B42" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="1">
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="1">
         <v>2023</v>
       </c>
-      <c r="B43" t="s">
-        <v>2</v>
-      </c>
-      <c r="C43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="1">
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="1">
         <v>2010</v>
       </c>
-      <c r="B44" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" s="1">
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="1">
         <v>1091</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="1">
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="1">
         <v>2011</v>
       </c>
-      <c r="B45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" s="1">
+      <c r="B48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="1">
         <v>498</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="1">
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
         <v>2012</v>
       </c>
-      <c r="B46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" s="1">
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="1">
         <v>972</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="1">
+      <c r="E49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
         <v>2013</v>
       </c>
-      <c r="B47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" t="s">
-        <v>7</v>
-      </c>
-      <c r="D47" s="1">
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="1">
         <v>1022</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="1">
+      <c r="E50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
         <v>2014</v>
       </c>
-      <c r="B48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" t="s">
-        <v>7</v>
-      </c>
-      <c r="D48" s="1">
+      <c r="B51" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="1">
         <v>1163</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="1">
+      <c r="E51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
         <v>2015</v>
       </c>
-      <c r="B49" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" s="1">
+      <c r="B52" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="1">
         <v>883</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="1">
+      <c r="E52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
         <v>2016</v>
       </c>
-      <c r="B50" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" s="1">
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="1">
         <v>578</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="1">
+      <c r="E53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="1">
         <v>2017</v>
       </c>
-      <c r="B51" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" s="1">
+      <c r="B54" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="1">
         <v>587</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="1">
+      <c r="E54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" s="1">
         <v>2018</v>
       </c>
-      <c r="B52" t="s">
-        <v>3</v>
-      </c>
-      <c r="C52" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="1">
+      <c r="B55" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="1">
         <v>626</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="1">
+      <c r="E55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" s="1">
         <v>2019</v>
       </c>
-      <c r="B53" t="s">
-        <v>3</v>
-      </c>
-      <c r="C53" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="1">
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="1">
         <v>469</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="1">
+      <c r="E56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="1">
         <v>2020</v>
       </c>
-      <c r="B54" t="s">
-        <v>3</v>
-      </c>
-      <c r="C54" t="s">
-        <v>7</v>
-      </c>
-      <c r="D54" s="1">
+      <c r="B57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="1">
         <v>420</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="1">
+      <c r="E57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" s="1">
         <v>2021</v>
       </c>
-      <c r="B55" t="s">
-        <v>3</v>
-      </c>
-      <c r="C55" t="s">
-        <v>7</v>
-      </c>
-      <c r="D55" s="1">
+      <c r="B58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="1">
         <v>507</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="1">
+      <c r="E58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" s="1">
         <v>2022</v>
       </c>
-      <c r="B56" t="s">
-        <v>3</v>
-      </c>
-      <c r="C56" t="s">
-        <v>7</v>
-      </c>
-      <c r="D56" s="1">
+      <c r="B59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="1">
         <v>535</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" s="1">
+      <c r="E59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" s="1">
         <v>2023</v>
       </c>
-      <c r="B57" t="s">
-        <v>3</v>
-      </c>
-      <c r="C57" t="s">
-        <v>7</v>
-      </c>
-      <c r="D57" s="1">
+      <c r="B60" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="1">
         <v>942</v>
+      </c>
+      <c r="E60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B61" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="1">
+        <v>718</v>
+      </c>
+      <c r="E61" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>